<commit_message>
Board almost completely drawn
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keena\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keena\Desktop\Clue\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{70A91E7B-178F-449B-B9E9-AE9D0950158F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD3799A-CC6B-4E7D-99FD-F40ECA81DDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F5C2579-9D7B-4A45-BA41-FF580A03F3F8}"/>
   </bookViews>
@@ -2602,11 +2602,11 @@
       <c r="AB21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AC21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="AD21" s="7" t="s">
+      <c r="AC21" s="7" t="s">
         <v>22</v>
+      </c>
+      <c r="AD21" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="AE21" s="3" t="s">
         <v>10</v>
@@ -2682,11 +2682,11 @@
       <c r="V22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W22" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="X22" s="7" t="s">
+      <c r="W22" s="7" t="s">
         <v>23</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="Y22" s="3" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Final touches for C23A
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keena\Desktop\Clue\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FD3799A-CC6B-4E7D-99FD-F40ECA81DDFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5A27CD-52FC-4A37-AA81-0715AFC27B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F5C2579-9D7B-4A45-BA41-FF580A03F3F8}"/>
+    <workbookView xWindow="3135" yWindow="2490" windowWidth="21600" windowHeight="11295" xr2:uid="{7F5C2579-9D7B-4A45-BA41-FF580A03F3F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -552,7 +552,7 @@
   <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AK21" sqref="AK21"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,8 +763,8 @@
       <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>15</v>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>7</v>
@@ -864,8 +864,8 @@
       <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>7</v>
+      <c r="E4" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
@@ -888,8 +888,8 @@
       <c r="L4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="7" t="s">
-        <v>18</v>
+      <c r="M4" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>5</v>
@@ -1277,8 +1277,8 @@
       <c r="K8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>5</v>
+      <c r="L8" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>5</v>
@@ -1939,8 +1939,8 @@
       <c r="C15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="7" t="s">
-        <v>16</v>
+      <c r="D15" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>2</v>
@@ -2153,8 +2153,8 @@
       <c r="I17" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="J17" s="3" t="s">
-        <v>2</v>
+      <c r="J17" s="7" t="s">
+        <v>16</v>
       </c>
       <c r="K17" s="3" t="s">
         <v>2</v>
@@ -2504,8 +2504,8 @@
       <c r="AB20" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AC20" s="3" t="s">
-        <v>10</v>
+      <c r="AC20" s="7" t="s">
+        <v>22</v>
       </c>
       <c r="AD20" s="3" t="s">
         <v>10</v>
@@ -2602,8 +2602,8 @@
       <c r="AB21" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="AC21" s="7" t="s">
-        <v>22</v>
+      <c r="AC21" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="AD21" s="3" t="s">
         <v>10</v>
@@ -2625,8 +2625,8 @@
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>17</v>
+      <c r="D22" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>9</v>
@@ -2658,8 +2658,8 @@
       <c r="N22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O22" s="8" t="s">
-        <v>19</v>
+      <c r="O22" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>8</v>
@@ -2821,8 +2821,8 @@
       <c r="C24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="3" t="s">
-        <v>9</v>
+      <c r="D24" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>9</v>
@@ -2854,8 +2854,8 @@
       <c r="N24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O24" s="5" t="s">
-        <v>8</v>
+      <c r="O24" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
Refactored text sizing in GUI
</commit_message>
<xml_diff>
--- a/data/ClueLayout.xlsx
+++ b/data/ClueLayout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keena\Desktop\Clue\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F5A27CD-52FC-4A37-AA81-0715AFC27B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D30DAC0A-D203-440C-8D9D-1EFD2313167D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3135" yWindow="2490" windowWidth="21600" windowHeight="11295" xr2:uid="{7F5C2579-9D7B-4A45-BA41-FF580A03F3F8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7F5C2579-9D7B-4A45-BA41-FF580A03F3F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -552,7 +552,7 @@
   <dimension ref="A1:AF37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,8 +766,8 @@
       <c r="D3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>7</v>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>7</v>
@@ -864,8 +864,8 @@
       <c r="D4" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="7" t="s">
-        <v>15</v>
+      <c r="E4" s="3" t="s">
+        <v>7</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>7</v>
@@ -921,14 +921,14 @@
       <c r="W4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="X4" s="5" t="s">
-        <v>4</v>
+      <c r="X4" s="8" t="s">
+        <v>20</v>
       </c>
       <c r="Y4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="Z4" s="8" t="s">
-        <v>20</v>
+      <c r="Z4" s="5" t="s">
+        <v>4</v>
       </c>
       <c r="AA4" s="5" t="s">
         <v>4</v>
@@ -1708,14 +1708,14 @@
       <c r="X12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="Y12" s="3" t="s">
-        <v>6</v>
+      <c r="Y12" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="Z12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA12" s="7" t="s">
-        <v>21</v>
+      <c r="AA12" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="AB12" s="3" t="s">
         <v>6</v>
@@ -2584,8 +2584,8 @@
       <c r="V21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W21" s="3" t="s">
-        <v>3</v>
+      <c r="W21" s="7" t="s">
+        <v>23</v>
       </c>
       <c r="X21" s="3" t="s">
         <v>3</v>
@@ -2625,8 +2625,8 @@
       <c r="C22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>9</v>
+      <c r="D22" s="7" t="s">
+        <v>17</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>9</v>
@@ -2658,8 +2658,8 @@
       <c r="N22" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O22" s="5" t="s">
-        <v>8</v>
+      <c r="O22" s="8" t="s">
+        <v>19</v>
       </c>
       <c r="P22" s="5" t="s">
         <v>8</v>
@@ -2682,8 +2682,8 @@
       <c r="V22" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="W22" s="7" t="s">
-        <v>23</v>
+      <c r="W22" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="X22" s="3" t="s">
         <v>3</v>
@@ -2821,8 +2821,8 @@
       <c r="C24" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>17</v>
+      <c r="D24" s="3" t="s">
+        <v>9</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>9</v>
@@ -2854,8 +2854,8 @@
       <c r="N24" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O24" s="8" t="s">
-        <v>19</v>
+      <c r="O24" s="5" t="s">
+        <v>8</v>
       </c>
       <c r="P24" s="5" t="s">
         <v>8</v>

</xml_diff>